<commit_message>
Update Buff Icon and Change buildAvatar
</commit_message>
<xml_diff>
--- a/GameDesign/ExcelData/Buff_Data.xlsx
+++ b/GameDesign/ExcelData/Buff_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\University\ucsc\GAME 271\project-Nameless Hill\NamelessHill-makeEnd\Nameless_Temp\GameDesign\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CA95B8-B184-4300-B6BB-F53A5C1570D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229C99D4-2C40-4F1A-BA41-34EEE16DE540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -419,7 +419,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>